<commit_message>
Add csv with category
</commit_message>
<xml_diff>
--- a/resources/startups.xlsx
+++ b/resources/startups.xlsx
@@ -1,36 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiomeurerpaitra/Documents/Plug Creative/Plug/Habitat Bradesco/InovaBra/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevend/coding/fabio/InovaBra/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACF8F87-BE6A-3B41-9052-A369348CA481}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="440" windowWidth="38400" windowHeight="22420"/>
+    <workbookView xWindow="25600" yWindow="440" windowWidth="38400" windowHeight="21160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Junho_18" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1086" uniqueCount="844">
   <si>
     <t>Nome</t>
   </si>
@@ -2541,12 +2542,33 @@
   </si>
   <si>
     <t>adriano.melito@myfirstipo.com.br</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Group 2</t>
+  </si>
+  <si>
+    <t>Group 1</t>
+  </si>
+  <si>
+    <t>Group 3</t>
+  </si>
+  <si>
+    <t>Group 4</t>
+  </si>
+  <si>
+    <t>Group 5</t>
+  </si>
+  <si>
+    <t>Group 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2928,11 +2950,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H136"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2948,7 +2970,7 @@
     <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2973,8 +2995,11 @@
       <c r="H1" s="3" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>114</v>
       </c>
@@ -2999,8 +3024,11 @@
       <c r="H2" s="1" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -3025,8 +3053,11 @@
       <c r="H3" s="1" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -3051,8 +3082,11 @@
       <c r="H4" s="1" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>432</v>
       </c>
@@ -3077,8 +3111,11 @@
       <c r="H5" s="1" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3103,8 +3140,11 @@
       <c r="H6" s="1" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -3129,8 +3169,11 @@
       <c r="H7" s="1" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -3155,8 +3198,11 @@
       <c r="H8" s="1" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3181,8 +3227,11 @@
       <c r="H9" s="1" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -3207,8 +3256,11 @@
       <c r="H10" s="1" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -3233,8 +3285,11 @@
       <c r="H11" s="1" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="I11" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -3259,8 +3314,11 @@
       <c r="H12" s="1" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="I12" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -3285,8 +3343,11 @@
       <c r="H13" s="1" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I13" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -3311,8 +3372,11 @@
       <c r="H14" s="1" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
@@ -3337,8 +3401,11 @@
       <c r="H15" s="1" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -3363,8 +3430,11 @@
       <c r="H16" s="1" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I16" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>113</v>
       </c>
@@ -3389,8 +3459,11 @@
       <c r="H17" s="1" t="s">
         <v>814</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -3415,8 +3488,11 @@
       <c r="H18" s="1" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="I18" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -3441,8 +3517,11 @@
       <c r="H19" s="1" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>459</v>
       </c>
@@ -3467,8 +3546,11 @@
       <c r="H20" s="1" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -3493,8 +3575,11 @@
       <c r="H21" s="1" t="s">
         <v>832</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -3519,8 +3604,11 @@
       <c r="H22" s="1" t="s">
         <v>833</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I22" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -3545,8 +3633,11 @@
       <c r="H23" s="1" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -3571,8 +3662,11 @@
       <c r="H24" s="1" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
@@ -3597,8 +3691,11 @@
       <c r="H25" s="1" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
@@ -3623,8 +3720,11 @@
       <c r="H26" s="1" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>112</v>
       </c>
@@ -3649,8 +3749,11 @@
       <c r="H27" s="1" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>111</v>
       </c>
@@ -3675,8 +3778,11 @@
       <c r="H28" s="1" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -3701,8 +3807,11 @@
       <c r="H29" s="1" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I29" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -3727,8 +3836,11 @@
       <c r="H30" s="1" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -3753,8 +3865,11 @@
       <c r="H31" s="1" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -3779,8 +3894,11 @@
       <c r="H32" s="1" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -3805,8 +3923,11 @@
       <c r="H33" s="1" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I33" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -3831,8 +3952,11 @@
       <c r="H34" s="1" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -3857,8 +3981,11 @@
       <c r="H35" s="1" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>110</v>
       </c>
@@ -3883,8 +4010,11 @@
       <c r="H36" s="1" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I36" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -3909,8 +4039,11 @@
       <c r="H37" s="1" t="s">
         <v>820</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -3935,8 +4068,11 @@
       <c r="H38" s="1" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I38" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -3961,8 +4097,11 @@
       <c r="H39" s="1" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>486</v>
       </c>
@@ -3987,8 +4126,11 @@
       <c r="H40" s="1" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I40" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>109</v>
       </c>
@@ -4013,8 +4155,11 @@
       <c r="H41" s="1" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>37</v>
       </c>
@@ -4039,8 +4184,11 @@
       <c r="H42" s="1" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>496</v>
       </c>
@@ -4065,8 +4213,11 @@
       <c r="H43" s="1" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>38</v>
       </c>
@@ -4091,8 +4242,11 @@
       <c r="H44" s="1" t="s">
         <v>812</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>39</v>
       </c>
@@ -4117,8 +4271,11 @@
       <c r="H45" s="1" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
@@ -4143,8 +4300,11 @@
       <c r="H46" s="1" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
@@ -4169,8 +4329,11 @@
       <c r="H47" s="1" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I47" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
@@ -4195,8 +4358,11 @@
       <c r="H48" s="1" t="s">
         <v>821</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>43</v>
       </c>
@@ -4221,8 +4387,11 @@
       <c r="H49" s="1" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>44</v>
       </c>
@@ -4247,8 +4416,11 @@
       <c r="H50" s="1" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I50" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
@@ -4273,8 +4445,11 @@
       <c r="H51" s="1" t="s">
         <v>835</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>108</v>
       </c>
@@ -4299,8 +4474,11 @@
       <c r="H52" s="1" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I52" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>46</v>
       </c>
@@ -4325,8 +4503,11 @@
       <c r="H53" s="1" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>506</v>
       </c>
@@ -4351,8 +4532,11 @@
       <c r="H54" s="1" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>47</v>
       </c>
@@ -4377,8 +4561,11 @@
       <c r="H55" s="1" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="I55" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
@@ -4403,8 +4590,11 @@
       <c r="H56" s="1" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>107</v>
       </c>
@@ -4429,8 +4619,11 @@
       <c r="H57" s="1" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>49</v>
       </c>
@@ -4455,8 +4648,11 @@
       <c r="H58" s="1" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I58" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>106</v>
       </c>
@@ -4481,8 +4677,11 @@
       <c r="H59" s="1" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I59" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>105</v>
       </c>
@@ -4507,8 +4706,11 @@
       <c r="H60" s="1" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>518</v>
       </c>
@@ -4533,8 +4735,11 @@
       <c r="H61" s="1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="I61" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>50</v>
       </c>
@@ -4559,8 +4764,11 @@
       <c r="H62" s="1" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I62" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>51</v>
       </c>
@@ -4585,8 +4793,11 @@
       <c r="H63" s="1" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>52</v>
       </c>
@@ -4611,8 +4822,11 @@
       <c r="H64" s="1" t="s">
         <v>834</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>53</v>
       </c>
@@ -4637,8 +4851,11 @@
       <c r="H65" s="1" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>54</v>
       </c>
@@ -4663,8 +4880,11 @@
       <c r="H66" s="1" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>55</v>
       </c>
@@ -4689,8 +4909,11 @@
       <c r="H67" s="1" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>56</v>
       </c>
@@ -4715,8 +4938,11 @@
       <c r="H68" s="1" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I68" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>57</v>
       </c>
@@ -4741,8 +4967,11 @@
       <c r="H69" s="1" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>104</v>
       </c>
@@ -4767,8 +4996,11 @@
       <c r="H70" s="1" t="s">
         <v>822</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>297</v>
       </c>
@@ -4793,8 +5025,11 @@
       <c r="H71" s="1" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>58</v>
       </c>
@@ -4819,8 +5054,11 @@
       <c r="H72" s="1" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I72" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>59</v>
       </c>
@@ -4845,8 +5083,11 @@
       <c r="H73" s="1" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="I73" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>60</v>
       </c>
@@ -4868,8 +5109,11 @@
       <c r="H74" s="1" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" s="1" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>61</v>
       </c>
@@ -4894,8 +5138,11 @@
       <c r="H75" s="1" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>62</v>
       </c>
@@ -4920,8 +5167,11 @@
       <c r="H76" s="1" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>63</v>
       </c>
@@ -4946,8 +5196,11 @@
       <c r="H77" s="1" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>64</v>
       </c>
@@ -4972,8 +5225,11 @@
       <c r="H78" s="1" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>65</v>
       </c>
@@ -4998,8 +5254,11 @@
       <c r="H79" s="1" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>66</v>
       </c>
@@ -5024,8 +5283,11 @@
       <c r="H80" s="1" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I80" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>67</v>
       </c>
@@ -5050,8 +5312,11 @@
       <c r="H81" s="1" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I81" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>68</v>
       </c>
@@ -5076,8 +5341,11 @@
       <c r="H82" s="1" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I82" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>546</v>
       </c>
@@ -5102,8 +5370,11 @@
       <c r="H83" s="1" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I83" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>551</v>
       </c>
@@ -5125,8 +5396,11 @@
       <c r="H84" s="1" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I84" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>103</v>
       </c>
@@ -5151,8 +5425,11 @@
       <c r="H85" s="1" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I85" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>559</v>
       </c>
@@ -5177,8 +5454,11 @@
       <c r="H86" s="1" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I86" s="1" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>564</v>
       </c>
@@ -5203,8 +5483,11 @@
       <c r="H87" s="1" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I87" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>102</v>
       </c>
@@ -5229,8 +5512,11 @@
       <c r="H88" s="1" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I88" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>101</v>
       </c>
@@ -5255,8 +5541,11 @@
       <c r="H89" s="1" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I89" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>69</v>
       </c>
@@ -5281,8 +5570,11 @@
       <c r="H90" s="1" t="s">
         <v>792</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I90" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>70</v>
       </c>
@@ -5307,8 +5599,11 @@
       <c r="H91" s="1" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I91" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>100</v>
       </c>
@@ -5333,8 +5628,11 @@
       <c r="H92" s="1" t="s">
         <v>819</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I92" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>71</v>
       </c>
@@ -5359,8 +5657,11 @@
       <c r="H93" s="1" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I93" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>72</v>
       </c>
@@ -5385,8 +5686,11 @@
       <c r="H94" s="1" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I94" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>73</v>
       </c>
@@ -5411,8 +5715,11 @@
       <c r="H95" s="1" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I95" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>74</v>
       </c>
@@ -5437,8 +5744,11 @@
       <c r="H96" s="1" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="I96" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>75</v>
       </c>
@@ -5463,8 +5773,11 @@
       <c r="H97" s="1" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I97" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>76</v>
       </c>
@@ -5489,8 +5802,11 @@
       <c r="H98" s="1" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I98" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>77</v>
       </c>
@@ -5515,8 +5831,11 @@
       <c r="H99" s="1" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+      <c r="I99" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>99</v>
       </c>
@@ -5538,8 +5857,11 @@
       <c r="H100" s="1" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I100" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>584</v>
       </c>
@@ -5564,8 +5886,11 @@
       <c r="H101" s="1" t="s">
         <v>817</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I101" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>98</v>
       </c>
@@ -5590,8 +5915,11 @@
       <c r="H102" s="1" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I102" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>592</v>
       </c>
@@ -5616,8 +5944,11 @@
       <c r="H103" s="1" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I103" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>78</v>
       </c>
@@ -5642,8 +5973,11 @@
       <c r="H104" s="1" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I104" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>79</v>
       </c>
@@ -5668,8 +6002,11 @@
       <c r="H105" s="1" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I105" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>80</v>
       </c>
@@ -5694,8 +6031,11 @@
       <c r="H106" s="1" t="s">
         <v>765</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I106" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>81</v>
       </c>
@@ -5720,8 +6060,11 @@
       <c r="H107" s="1" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I107" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>82</v>
       </c>
@@ -5746,8 +6089,11 @@
       <c r="H108" s="1" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I108" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>97</v>
       </c>
@@ -5772,8 +6118,11 @@
       <c r="H109" s="1" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I109" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>83</v>
       </c>
@@ -5798,8 +6147,11 @@
       <c r="H110" s="1" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I110" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>84</v>
       </c>
@@ -5824,8 +6176,11 @@
       <c r="H111" s="1" t="s">
         <v>768</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I111" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>85</v>
       </c>
@@ -5850,8 +6205,11 @@
       <c r="H112" s="1" t="s">
         <v>769</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I112" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>86</v>
       </c>
@@ -5876,8 +6234,11 @@
       <c r="H113" s="1" t="s">
         <v>770</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="60" x14ac:dyDescent="0.2">
+      <c r="I113" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>610</v>
       </c>
@@ -5902,8 +6263,11 @@
       <c r="H114" s="1" t="s">
         <v>771</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I114" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>615</v>
       </c>
@@ -5928,8 +6292,11 @@
       <c r="H115" s="1" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I115" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>87</v>
       </c>
@@ -5954,8 +6321,11 @@
       <c r="H116" s="1" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I116" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>88</v>
       </c>
@@ -5980,8 +6350,11 @@
       <c r="H117" s="1" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I117" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>89</v>
       </c>
@@ -6006,8 +6379,11 @@
       <c r="H118" s="1" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I118" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>90</v>
       </c>
@@ -6032,8 +6408,11 @@
       <c r="H119" s="1" t="s">
         <v>825</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I119" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>625</v>
       </c>
@@ -6058,8 +6437,11 @@
       <c r="H120" s="1" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="I120" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>91</v>
       </c>
@@ -6084,8 +6466,11 @@
       <c r="H121" s="1" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I121" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>92</v>
       </c>
@@ -6110,8 +6495,11 @@
       <c r="H122" s="1" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I122" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>93</v>
       </c>
@@ -6136,8 +6524,11 @@
       <c r="H123" s="1" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I123" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>632</v>
       </c>
@@ -6162,8 +6553,11 @@
       <c r="H124" s="1" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I124" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>96</v>
       </c>
@@ -6188,8 +6582,11 @@
       <c r="H125" s="1" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I125" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>640</v>
       </c>
@@ -6214,8 +6611,11 @@
       <c r="H126" s="1" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I126" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>94</v>
       </c>
@@ -6240,8 +6640,11 @@
       <c r="H127" s="1" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I127" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>95</v>
       </c>
@@ -6266,8 +6669,11 @@
       <c r="H128" s="1" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I128" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>646</v>
       </c>
@@ -6292,8 +6698,11 @@
       <c r="H129" s="1" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I129" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>652</v>
       </c>
@@ -6318,8 +6727,11 @@
       <c r="H130" s="1" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I130" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>657</v>
       </c>
@@ -6344,8 +6756,11 @@
       <c r="H131" s="1" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I131" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>662</v>
       </c>
@@ -6370,8 +6785,11 @@
       <c r="H132" s="1" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I132" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>668</v>
       </c>
@@ -6396,8 +6814,11 @@
       <c r="H133" s="1" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I133" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>684</v>
       </c>
@@ -6422,8 +6843,11 @@
       <c r="H134" s="1" t="s">
         <v>823</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I134" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>685</v>
       </c>
@@ -6448,8 +6872,11 @@
       <c r="H135" s="1" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I135" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>686</v>
       </c>
@@ -6474,28 +6901,31 @@
       <c r="H136" s="1" t="s">
         <v>786</v>
       </c>
+      <c r="I136" s="1" t="s">
+        <v>843</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G19" r:id="rId1"/>
-    <hyperlink ref="B20" r:id="rId2"/>
-    <hyperlink ref="G20" r:id="rId3"/>
-    <hyperlink ref="B30" r:id="rId4"/>
-    <hyperlink ref="B33" r:id="rId5"/>
-    <hyperlink ref="G35" r:id="rId6"/>
-    <hyperlink ref="B39" r:id="rId7"/>
-    <hyperlink ref="B40" r:id="rId8"/>
-    <hyperlink ref="G40" r:id="rId9"/>
-    <hyperlink ref="G41" r:id="rId10"/>
-    <hyperlink ref="G63" r:id="rId11"/>
-    <hyperlink ref="G67" r:id="rId12"/>
-    <hyperlink ref="G68" r:id="rId13"/>
-    <hyperlink ref="G85" r:id="rId14"/>
-    <hyperlink ref="G91" r:id="rId15"/>
-    <hyperlink ref="G109" r:id="rId16"/>
-    <hyperlink ref="G128" r:id="rId17"/>
-    <hyperlink ref="G134" r:id="rId18"/>
-    <hyperlink ref="G33" r:id="rId19"/>
+    <hyperlink ref="G19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G20" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B30" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B33" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G35" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B39" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B40" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G40" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G41" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G63" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G67" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G68" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G85" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G91" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G109" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G128" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G134" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G33" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>